<commit_message>
Modify frm_match_100_test & Extensions
add SELECT_NODE()
SELECT_NODES()
CLASS()
TEXT()
E_TRIM()
E_SPLIT()
to Extension

add test_sportbet()
test_victorbet()
test_marathonbet()
test_coral()
function to frm_match_100_test

add sample() funtion to Match100Methd
</commit_message>
<xml_diff>
--- a/web_helper/data/sites/template.xlsx
+++ b/web_helper/data/sites/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>bet16</t>
   </si>
@@ -159,6 +159,78 @@
   </si>
   <si>
     <t>Aug 2902:45</t>
+  </si>
+  <si>
+    <t>sportbet</t>
+  </si>
+  <si>
+    <t>win  /div[2]/div[1]/div[1]/a[1]/span[2]</t>
+  </si>
+  <si>
+    <t>draw  /div[2]/div[1]/div[2]/a[1]/span[2]</t>
+  </si>
+  <si>
+    <t>lose  /div[2]/div[1]/div[3]/a[1]/span[2]</t>
+  </si>
+  <si>
+    <t>victorbet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /td[1]</t>
+  </si>
+  <si>
+    <t>teams</t>
+  </si>
+  <si>
+    <t>/td[2]/a[1]</t>
+  </si>
+  <si>
+    <t>/td[2]/span[1]</t>
+  </si>
+  <si>
+    <t>/td[3]/span[1]/a[1]/span[1]</t>
+  </si>
+  <si>
+    <t>/td[4]/span[1]/a[1]/span[1]</t>
+  </si>
+  <si>
+    <t>/td[5]/span[1]/a[1]/span[1]</t>
+  </si>
+  <si>
+    <t>marathonbet</t>
+  </si>
+  <si>
+    <t>div[1]/h2[1]</t>
+  </si>
+  <si>
+    <t>/tr[1]/td[1]/table[1]/tbody[1]/tr[1]/td[2]</t>
+  </si>
+  <si>
+    <t>div[2]/div[1]/table[1]/tbody</t>
+  </si>
+  <si>
+    <t>/tr[1]/td[1]/table[1]/tbody[1]/tr[1]/td[1]/span[1]/div[1]</t>
+  </si>
+  <si>
+    <t>/tr[1]/td[1]/table[1]/tbody[1]/tr[1]/td[1]/span[1]/div[2]</t>
+  </si>
+  <si>
+    <t>/tr[1]/td[2]</t>
+  </si>
+  <si>
+    <t>/tr[1]/td[3]</t>
+  </si>
+  <si>
+    <t>/tr[1]/td[4]</t>
+  </si>
+  <si>
+    <t>coral</t>
+  </si>
+  <si>
+    <t>/div[5]/div[1]/span[2]</t>
   </si>
 </sst>
 </file>
@@ -493,16 +565,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="84.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -716,14 +788,166 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new function to frm_match_100_method_test
add function to frm_match_100_method_test:
test_gamebookers()
test_oddstring()
test_snai()
test_12bet()
test_1bet()
test_youwin()
add new class P.cs
add new function E_REMOVE to Extentions.cs
</commit_message>
<xml_diff>
--- a/web_helper/data/sites/template.xlsx
+++ b/web_helper/data/sites/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
   <si>
     <t>bet16</t>
   </si>
@@ -231,6 +231,87 @@
   </si>
   <si>
     <t>/div[5]/div[1]/span[2]</t>
+  </si>
+  <si>
+    <t>gamebooker</t>
+  </si>
+  <si>
+    <t>/h6[1]/span[2]+h6[1]/span[1]</t>
+  </si>
+  <si>
+    <t>/tbody[1]/tr[1]/td[1]/button[1]/span[2]</t>
+  </si>
+  <si>
+    <t>/tbody[1]/tr[1]/td[1]/button[1]/span[1]</t>
+  </si>
+  <si>
+    <t>/tbody[1]/tr[1]/td[3]/button[1]/span[2]</t>
+  </si>
+  <si>
+    <t>/tbody[1]/tr[1]/td[2]/button[1]/span[1]</t>
+  </si>
+  <si>
+    <t>/tbody[1]/tr[1]/td[3]/button[1]/span[1]</t>
+  </si>
+  <si>
+    <t>oddring</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>/td[3]</t>
+  </si>
+  <si>
+    <t>/td[3]/div[1]</t>
+  </si>
+  <si>
+    <t>/td[3]/span[1]</t>
+  </si>
+  <si>
+    <t>/td[4]/div[1]/a[1]</t>
+  </si>
+  <si>
+    <t>12bet</t>
+  </si>
+  <si>
+    <t>/td[2]/span[2]</t>
+  </si>
+  <si>
+    <t>odds</t>
+  </si>
+  <si>
+    <t>/td[9]</t>
+  </si>
+  <si>
+    <t>1bet</t>
+  </si>
+  <si>
+    <t>start_Time</t>
+  </si>
+  <si>
+    <t>/td[1]/div[1]</t>
+  </si>
+  <si>
+    <t>youwin</t>
+  </si>
+  <si>
+    <t>tbody[1]/tr[1]/td[1]</t>
+  </si>
+  <si>
+    <t>tbody[1]/tr[1]/td[2]/div[1]</t>
+  </si>
+  <si>
+    <t>tbody[1]/tr[1]/td[2]/div[2]</t>
+  </si>
+  <si>
+    <t>tbody[1]/tr[1]/td[3]</t>
+  </si>
+  <si>
+    <t>tbody[1]/tr[1]/td[4]</t>
+  </si>
+  <si>
+    <t>tbody[1]/tr[1]/td[5]</t>
   </si>
 </sst>
 </file>
@@ -565,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -678,7 +759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="45">
+    <row r="23" spans="1:1" ht="120">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -948,6 +1029,231 @@
       </c>
       <c r="B81" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>54</v>
+      </c>
+      <c r="B94" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>86</v>
+      </c>
+      <c r="B102" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>89</v>
+      </c>
+      <c r="B105" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>54</v>
+      </c>
+      <c r="B106" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function to frm_match_100_method_test & add function to write_log when load data
add below:
test_youwage()
test_paddypower()
test_vwin()
test_betally()
test_18bet()
test_mcbookie()
test_betcenter()
tet_joinbet()
test_tonybet()
test_topsport()
add write_log to Match100Helper
</commit_message>
<xml_diff>
--- a/web_helper/data/sites/template.xlsx
+++ b/web_helper/data/sites/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
   <si>
     <t>bet16</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>tbody[1]/tr[1]/td[5]</t>
+  </si>
+  <si>
+    <t>youwage</t>
   </si>
 </sst>
 </file>
@@ -646,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1254,6 +1257,11 @@
       </c>
       <c r="B118" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>